<commit_message>
Add Requirements pdf for Lab3.
</commit_message>
<xml_diff>
--- a/Docs/Lab3/Lab03_BBT_TCs_Form.xlsx
+++ b/Docs/Lab3/Lab03_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F4ABEF-CF43-4184-BAED-4146ED851C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0371C9F7-0968-4A20-A201-B8F459B19B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="1752" windowWidth="17628" windowHeight="10320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cerinta" sheetId="1" r:id="rId1"/>
@@ -1616,6 +1616,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1643,77 +1647,95 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1721,23 +1743,47 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1751,12 +1797,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1766,9 +1806,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1790,46 +1827,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1860,7 +1860,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>255270</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:rowOff>178904</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1875,8 +1875,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="720090" y="891540"/>
-          <a:ext cx="6850380" cy="1337310"/>
+          <a:off x="720090" y="901148"/>
+          <a:ext cx="6850380" cy="1530626"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2634,8 +2634,8 @@
   </sheetPr>
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2646,12 +2646,12 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="119"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="121"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="L2" s="91" t="s">
@@ -2664,33 +2664,33 @@
       <c r="Q2" s="92"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="L3" s="120" t="s">
+      <c r="L3" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="121"/>
-      <c r="N3" s="122" t="s">
+      <c r="M3" s="123"/>
+      <c r="N3" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="123"/>
-      <c r="P3" s="123"/>
-      <c r="Q3" s="124"/>
+      <c r="O3" s="125"/>
+      <c r="P3" s="125"/>
+      <c r="Q3" s="126"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="L4" s="125" t="s">
+      <c r="L4" s="127" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="125"/>
+      <c r="M4" s="127"/>
       <c r="N4" s="75" t="s">
         <v>52</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="122">
+      <c r="P4" s="124">
         <v>1211</v>
       </c>
-      <c r="Q4" s="124"/>
+      <c r="Q4" s="126"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -2819,7 +2819,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="I16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -2845,12 +2845,12 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="119"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="121"/>
     </row>
     <row r="2" spans="2:17" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22"/>
@@ -2870,49 +2870,49 @@
       <c r="H3" s="90"/>
     </row>
     <row r="5" spans="2:17" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="140"/>
-      <c r="H5" s="141" t="s">
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="H5" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="141"/>
-      <c r="J5" s="141"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
     </row>
     <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="140"/>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="142"/>
-      <c r="J6" s="142"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G7" s="143" t="s">
+      <c r="G7" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="145" t="s">
+      <c r="H7" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="132" t="s">
+      <c r="I7" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="133"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="134"/>
-      <c r="P7" s="135" t="s">
+      <c r="J7" s="145"/>
+      <c r="K7" s="145"/>
+      <c r="L7" s="145"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="145"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="135"/>
+      <c r="Q7" s="147"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
@@ -2927,8 +2927,8 @@
       <c r="E8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="144"/>
-      <c r="H8" s="146"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="136"/>
       <c r="I8" s="14" t="s">
         <v>67</v>
       </c>
@@ -2944,20 +2944,20 @@
       <c r="M8" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="N8" s="132" t="s">
+      <c r="N8" s="144" t="s">
         <v>72</v>
       </c>
-      <c r="O8" s="134"/>
-      <c r="P8" s="132" t="s">
+      <c r="O8" s="146"/>
+      <c r="P8" s="144" t="s">
         <v>7</v>
       </c>
-      <c r="Q8" s="134"/>
+      <c r="Q8" s="146"/>
     </row>
     <row r="9" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="84">
         <v>1</v>
       </c>
-      <c r="C9" s="147" t="s">
+      <c r="C9" s="137" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="98" t="s">
@@ -2985,20 +2985,20 @@
       <c r="M9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="126">
+      <c r="N9" s="140">
         <v>3000</v>
       </c>
-      <c r="O9" s="127"/>
-      <c r="P9" s="130" t="s">
+      <c r="O9" s="141"/>
+      <c r="P9" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="Q9" s="131"/>
+      <c r="Q9" s="143"/>
     </row>
     <row r="10" spans="2:17" s="66" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="84">
         <v>2</v>
       </c>
-      <c r="C10" s="148"/>
+      <c r="C10" s="138"/>
       <c r="D10" s="98"/>
       <c r="E10" s="99" t="s">
         <v>56</v>
@@ -3037,7 +3037,7 @@
       <c r="B11" s="84">
         <v>3</v>
       </c>
-      <c r="C11" s="148"/>
+      <c r="C11" s="138"/>
       <c r="D11" s="97"/>
       <c r="E11" s="99" t="s">
         <v>58</v>
@@ -3076,7 +3076,7 @@
       <c r="B12" s="84">
         <v>4</v>
       </c>
-      <c r="C12" s="149"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="84"/>
       <c r="E12" s="99" t="s">
         <v>57</v>
@@ -3102,20 +3102,20 @@
       <c r="M12" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N12" s="126">
+      <c r="N12" s="140">
         <v>3000</v>
       </c>
-      <c r="O12" s="127"/>
-      <c r="P12" s="136" t="s">
+      <c r="O12" s="141"/>
+      <c r="P12" s="148" t="s">
         <v>80</v>
       </c>
-      <c r="Q12" s="137"/>
+      <c r="Q12" s="149"/>
     </row>
     <row r="13" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="84">
         <v>5</v>
       </c>
-      <c r="C13" s="147" t="s">
+      <c r="C13" s="137" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="98" t="s">
@@ -3145,20 +3145,20 @@
       <c r="M13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N13" s="126">
+      <c r="N13" s="140">
         <v>3000</v>
       </c>
-      <c r="O13" s="127"/>
-      <c r="P13" s="136" t="s">
+      <c r="O13" s="141"/>
+      <c r="P13" s="148" t="s">
         <v>80</v>
       </c>
-      <c r="Q13" s="127"/>
+      <c r="Q13" s="141"/>
     </row>
     <row r="14" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="84">
         <v>6</v>
       </c>
-      <c r="C14" s="149"/>
+      <c r="C14" s="139"/>
       <c r="D14" s="84"/>
       <c r="E14" s="99"/>
       <c r="G14" s="21">
@@ -3170,16 +3170,16 @@
       <c r="K14" s="20"/>
       <c r="L14" s="38"/>
       <c r="M14" s="20"/>
-      <c r="N14" s="126"/>
-      <c r="O14" s="127"/>
-      <c r="P14" s="126"/>
-      <c r="Q14" s="127"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="141"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="141"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="84">
         <v>7</v>
       </c>
-      <c r="C15" s="138"/>
+      <c r="C15" s="128"/>
       <c r="D15" s="84"/>
       <c r="E15" s="84"/>
       <c r="G15" s="21">
@@ -3191,16 +3191,16 @@
       <c r="K15" s="20"/>
       <c r="L15" s="38"/>
       <c r="M15" s="20"/>
-      <c r="N15" s="126"/>
-      <c r="O15" s="127"/>
-      <c r="P15" s="126"/>
-      <c r="Q15" s="127"/>
+      <c r="N15" s="140"/>
+      <c r="O15" s="141"/>
+      <c r="P15" s="140"/>
+      <c r="Q15" s="141"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="84">
         <v>8</v>
       </c>
-      <c r="C16" s="139"/>
+      <c r="C16" s="129"/>
       <c r="D16" s="84"/>
       <c r="E16" s="84"/>
       <c r="G16" s="21">
@@ -3212,16 +3212,16 @@
       <c r="K16" s="20"/>
       <c r="L16" s="38"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="126"/>
-      <c r="O16" s="127"/>
-      <c r="P16" s="126"/>
-      <c r="Q16" s="127"/>
+      <c r="N16" s="140"/>
+      <c r="O16" s="141"/>
+      <c r="P16" s="140"/>
+      <c r="Q16" s="141"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" s="84">
         <v>9</v>
       </c>
-      <c r="C17" s="138"/>
+      <c r="C17" s="128"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
       <c r="G17" s="21">
@@ -3233,16 +3233,16 @@
       <c r="K17" s="20"/>
       <c r="L17" s="38"/>
       <c r="M17" s="20"/>
-      <c r="N17" s="126"/>
-      <c r="O17" s="127"/>
-      <c r="P17" s="130"/>
-      <c r="Q17" s="131"/>
+      <c r="N17" s="140"/>
+      <c r="O17" s="141"/>
+      <c r="P17" s="142"/>
+      <c r="Q17" s="143"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B18" s="84">
         <v>10</v>
       </c>
-      <c r="C18" s="139"/>
+      <c r="C18" s="129"/>
       <c r="D18" s="84"/>
       <c r="E18" s="84"/>
       <c r="G18" s="21"/>
@@ -3252,16 +3252,16 @@
       <c r="K18" s="20"/>
       <c r="L18" s="38"/>
       <c r="M18" s="20"/>
-      <c r="N18" s="126"/>
-      <c r="O18" s="127"/>
-      <c r="P18" s="126"/>
-      <c r="Q18" s="127"/>
+      <c r="N18" s="140"/>
+      <c r="O18" s="141"/>
+      <c r="P18" s="140"/>
+      <c r="Q18" s="141"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="84">
         <v>11</v>
       </c>
-      <c r="C19" s="138"/>
+      <c r="C19" s="128"/>
       <c r="D19" s="84"/>
       <c r="E19" s="84"/>
       <c r="G19" s="11"/>
@@ -3271,16 +3271,16 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="126"/>
-      <c r="O19" s="127"/>
-      <c r="P19" s="128"/>
-      <c r="Q19" s="129"/>
+      <c r="N19" s="140"/>
+      <c r="O19" s="141"/>
+      <c r="P19" s="150"/>
+      <c r="Q19" s="151"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" s="84">
         <v>12</v>
       </c>
-      <c r="C20" s="139"/>
+      <c r="C20" s="129"/>
       <c r="D20" s="84"/>
       <c r="E20" s="84"/>
       <c r="G20" s="11"/>
@@ -3290,16 +3290,16 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="126"/>
-      <c r="O20" s="127"/>
-      <c r="P20" s="128"/>
-      <c r="Q20" s="129"/>
+      <c r="N20" s="140"/>
+      <c r="O20" s="141"/>
+      <c r="P20" s="150"/>
+      <c r="Q20" s="151"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="84">
         <v>13</v>
       </c>
-      <c r="C21" s="138"/>
+      <c r="C21" s="128"/>
       <c r="D21" s="84"/>
       <c r="E21" s="84"/>
       <c r="G21" s="11"/>
@@ -3309,16 +3309,16 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="126"/>
-      <c r="O21" s="127"/>
-      <c r="P21" s="128"/>
-      <c r="Q21" s="129"/>
+      <c r="N21" s="140"/>
+      <c r="O21" s="141"/>
+      <c r="P21" s="150"/>
+      <c r="Q21" s="151"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" s="84">
         <v>14</v>
       </c>
-      <c r="C22" s="139"/>
+      <c r="C22" s="129"/>
       <c r="D22" s="84"/>
       <c r="E22" s="84"/>
       <c r="G22" s="14"/>
@@ -3328,16 +3328,16 @@
       <c r="K22" s="20"/>
       <c r="L22" s="38"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="126"/>
-      <c r="O22" s="127"/>
-      <c r="P22" s="128"/>
-      <c r="Q22" s="129"/>
+      <c r="N22" s="140"/>
+      <c r="O22" s="141"/>
+      <c r="P22" s="150"/>
+      <c r="Q22" s="151"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" s="84">
         <v>15</v>
       </c>
-      <c r="C23" s="138"/>
+      <c r="C23" s="128"/>
       <c r="D23" s="84"/>
       <c r="E23" s="84"/>
     </row>
@@ -3345,7 +3345,7 @@
       <c r="B24" s="84">
         <v>16</v>
       </c>
-      <c r="C24" s="139"/>
+      <c r="C24" s="129"/>
       <c r="D24" s="84"/>
       <c r="E24" s="84"/>
     </row>
@@ -3452,18 +3452,18 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="H5:J6"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="P17:Q17"/>
@@ -3480,18 +3480,18 @@
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N13:O13"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="H5:J6"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3534,12 +3534,12 @@
       <c r="B1" s="22"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="117" t="s">
+      <c r="E1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="119"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="121"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C2" s="77" t="s">
@@ -3556,57 +3556,57 @@
       <c r="J4" s="77"/>
     </row>
     <row r="5" spans="2:18" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="155" t="s">
+      <c r="B5" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="H5" s="141" t="s">
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="H5" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="141"/>
-      <c r="J5" s="141"/>
-      <c r="K5" s="141"/>
-      <c r="L5" s="141"/>
-      <c r="M5" s="141"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="131"/>
+      <c r="M5" s="131"/>
     </row>
     <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="156"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="157"/>
+      <c r="E6" s="157"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-      <c r="H6" s="141"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="141"/>
-      <c r="K6" s="141"/>
-      <c r="L6" s="141"/>
-      <c r="M6" s="141"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="131"/>
+      <c r="M6" s="131"/>
     </row>
     <row r="7" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F7" s="5"/>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="143" t="s">
+      <c r="I7" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="143" t="s">
+      <c r="J7" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="145" t="s">
+      <c r="K7" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="152" t="s">
+      <c r="L7" s="153" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="153"/>
-      <c r="N7" s="153"/>
-      <c r="O7" s="153"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="154"/>
+      <c r="M7" s="154"/>
+      <c r="N7" s="154"/>
+      <c r="O7" s="154"/>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="155"/>
       <c r="R7" s="86" t="s">
         <v>6</v>
       </c>
@@ -3618,15 +3618,15 @@
       <c r="C8" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="132" t="s">
+      <c r="D8" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="134"/>
+      <c r="E8" s="146"/>
       <c r="F8" s="3"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="144"/>
-      <c r="J8" s="144"/>
-      <c r="K8" s="146"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="136"/>
       <c r="L8" s="30" t="s">
         <v>67</v>
       </c>
@@ -3650,10 +3650,10 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="138" t="s">
+      <c r="B9" s="128" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="147" t="s">
+      <c r="C9" s="137" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="84">
@@ -3698,8 +3698,8 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="157"/>
-      <c r="C10" s="148"/>
+      <c r="B10" s="152"/>
+      <c r="C10" s="138"/>
       <c r="D10" s="84">
         <v>2</v>
       </c>
@@ -3742,8 +3742,8 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="157"/>
-      <c r="C11" s="148"/>
+      <c r="B11" s="152"/>
+      <c r="C11" s="138"/>
       <c r="D11" s="84">
         <v>3</v>
       </c>
@@ -3786,8 +3786,8 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="157"/>
-      <c r="C12" s="148"/>
+      <c r="B12" s="152"/>
+      <c r="C12" s="138"/>
       <c r="D12" s="84">
         <v>4</v>
       </c>
@@ -3810,8 +3810,8 @@
       <c r="R12" s="71"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="157"/>
-      <c r="C13" s="148"/>
+      <c r="B13" s="152"/>
+      <c r="C13" s="138"/>
       <c r="D13" s="84">
         <v>5</v>
       </c>
@@ -3834,8 +3834,8 @@
       <c r="R13" s="71"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="139"/>
-      <c r="C14" s="149"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="139"/>
       <c r="D14" s="84">
         <v>6</v>
       </c>
@@ -3858,10 +3858,10 @@
       <c r="R14" s="71"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="147" t="s">
+      <c r="C15" s="137" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="84">
@@ -3906,8 +3906,8 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="157"/>
-      <c r="C16" s="148"/>
+      <c r="B16" s="152"/>
+      <c r="C16" s="138"/>
       <c r="D16" s="84">
         <v>8</v>
       </c>
@@ -3950,8 +3950,8 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="157"/>
-      <c r="C17" s="148"/>
+      <c r="B17" s="152"/>
+      <c r="C17" s="138"/>
       <c r="D17" s="84">
         <v>9</v>
       </c>
@@ -3994,8 +3994,8 @@
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="157"/>
-      <c r="C18" s="148"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="138"/>
       <c r="D18" s="84">
         <v>10</v>
       </c>
@@ -4038,8 +4038,8 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="157"/>
-      <c r="C19" s="148"/>
+      <c r="B19" s="152"/>
+      <c r="C19" s="138"/>
       <c r="D19" s="84">
         <v>11</v>
       </c>
@@ -4062,8 +4062,8 @@
       <c r="R19" s="71"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="139"/>
-      <c r="C20" s="149"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="139"/>
       <c r="D20" s="84">
         <v>12</v>
       </c>
@@ -4086,10 +4086,10 @@
       <c r="R20" s="72"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="138"/>
+      <c r="C21" s="128"/>
       <c r="D21" s="84">
         <v>13</v>
       </c>
@@ -4112,8 +4112,8 @@
       <c r="R21" s="72"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="157"/>
-      <c r="C22" s="157"/>
+      <c r="B22" s="152"/>
+      <c r="C22" s="152"/>
       <c r="D22" s="84">
         <v>14</v>
       </c>
@@ -4136,8 +4136,8 @@
       <c r="R22" s="72"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="157"/>
-      <c r="C23" s="157"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
       <c r="D23" s="84">
         <v>15</v>
       </c>
@@ -4160,8 +4160,8 @@
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="152"/>
       <c r="D24" s="84">
         <v>16</v>
       </c>
@@ -4184,8 +4184,8 @@
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="157"/>
-      <c r="C25" s="157"/>
+      <c r="B25" s="152"/>
+      <c r="C25" s="152"/>
       <c r="D25" s="84">
         <v>17</v>
       </c>
@@ -4208,8 +4208,8 @@
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="139"/>
-      <c r="C26" s="139"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
       <c r="D26" s="84">
         <v>18</v>
       </c>
@@ -4232,10 +4232,10 @@
       <c r="R26" s="72"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="138" t="s">
+      <c r="B27" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="138"/>
+      <c r="C27" s="128"/>
       <c r="D27" s="84">
         <v>19</v>
       </c>
@@ -4259,8 +4259,8 @@
       <c r="S27" s="3"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B28" s="157"/>
-      <c r="C28" s="157"/>
+      <c r="B28" s="152"/>
+      <c r="C28" s="152"/>
       <c r="D28" s="84">
         <v>20</v>
       </c>
@@ -4284,8 +4284,8 @@
       <c r="S28" s="3"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="157"/>
-      <c r="C29" s="157"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="152"/>
       <c r="D29" s="84">
         <v>21</v>
       </c>
@@ -4309,8 +4309,8 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B30" s="157"/>
-      <c r="C30" s="157"/>
+      <c r="B30" s="152"/>
+      <c r="C30" s="152"/>
       <c r="D30" s="84">
         <v>22</v>
       </c>
@@ -4334,8 +4334,8 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
+      <c r="B31" s="152"/>
+      <c r="C31" s="152"/>
       <c r="D31" s="84">
         <v>23</v>
       </c>
@@ -4358,8 +4358,8 @@
       <c r="R31" s="71"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="139"/>
-      <c r="C32" s="139"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="129"/>
       <c r="D32" s="84">
         <v>24</v>
       </c>
@@ -4381,10 +4381,10 @@
       <c r="R32" s="72"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B33" s="138" t="s">
+      <c r="B33" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="138"/>
+      <c r="C33" s="128"/>
       <c r="D33" s="84">
         <v>25</v>
       </c>
@@ -4406,8 +4406,8 @@
       <c r="R33" s="87"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B34" s="157"/>
-      <c r="C34" s="157"/>
+      <c r="B34" s="152"/>
+      <c r="C34" s="152"/>
       <c r="D34" s="84">
         <v>26</v>
       </c>
@@ -4429,8 +4429,8 @@
       <c r="R34" s="72"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="157"/>
-      <c r="C35" s="157"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
       <c r="D35" s="84">
         <v>27</v>
       </c>
@@ -4452,8 +4452,8 @@
       <c r="R35" s="71"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
+      <c r="B36" s="152"/>
+      <c r="C36" s="152"/>
       <c r="D36" s="84">
         <v>28</v>
       </c>
@@ -4475,8 +4475,8 @@
       <c r="R36" s="71"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B37" s="157"/>
-      <c r="C37" s="157"/>
+      <c r="B37" s="152"/>
+      <c r="C37" s="152"/>
       <c r="D37" s="84">
         <v>29</v>
       </c>
@@ -4498,8 +4498,8 @@
       <c r="R37" s="71"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="139"/>
-      <c r="C38" s="139"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="129"/>
       <c r="D38" s="84">
         <v>30</v>
       </c>
@@ -4524,8 +4524,8 @@
       <c r="A40" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="H40" s="150"/>
-      <c r="I40" s="151"/>
+      <c r="H40" s="158"/>
+      <c r="I40" s="159"/>
       <c r="J40" s="66"/>
       <c r="K40" s="66"/>
       <c r="L40" s="66"/>
@@ -4562,6 +4562,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="H5:M6"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="B33:B38"/>
@@ -4572,16 +4582,6 @@
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="C21:C26"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="L7:Q7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="H5:M6"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4596,7 +4596,7 @@
   </sheetPr>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+    <sheetView topLeftCell="B22" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -4618,12 +4618,12 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="119"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="2" spans="2:13" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22"/>
@@ -4634,20 +4634,20 @@
     </row>
     <row r="3" spans="2:13" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22"/>
-      <c r="C3" s="168" t="s">
+      <c r="C3" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="169"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="169"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="169"/>
+      <c r="C4" s="182"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="182"/>
+      <c r="G4" s="182"/>
       <c r="L4" s="115" t="s">
         <v>106</v>
       </c>
@@ -4656,33 +4656,33 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="175" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="145" t="s">
+      <c r="D5" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="132" t="s">
+      <c r="E5" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="134"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="145"/>
+      <c r="K5" s="146"/>
       <c r="L5" s="88" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="66"/>
     </row>
     <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="158"/>
-      <c r="C6" s="160"/>
-      <c r="D6" s="161"/>
+      <c r="B6" s="174"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="177"/>
       <c r="E6" s="16" t="s">
         <v>67</v>
       </c>
@@ -5326,81 +5326,81 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="164"/>
-      <c r="D34" s="164"/>
-      <c r="E34" s="165"/>
+      <c r="C34" s="178"/>
+      <c r="D34" s="178"/>
+      <c r="E34" s="179"/>
       <c r="F34" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="171" t="s">
+      <c r="G34" s="184" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="172"/>
-      <c r="I34" s="172"/>
-      <c r="J34" s="164"/>
-      <c r="K34" s="173"/>
-      <c r="L34" s="178" t="s">
+      <c r="H34" s="185"/>
+      <c r="I34" s="185"/>
+      <c r="J34" s="178"/>
+      <c r="K34" s="186"/>
+      <c r="L34" s="160" t="s">
         <v>25</v>
       </c>
-      <c r="M34" s="179"/>
-      <c r="N34" s="180"/>
+      <c r="M34" s="161"/>
+      <c r="N34" s="162"/>
     </row>
     <row r="35" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="66"/>
-      <c r="C35" s="166" t="s">
+      <c r="C35" s="180" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="166" t="s">
+      <c r="D35" s="180" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="167" t="s">
+      <c r="E35" s="164" t="s">
         <v>21</v>
       </c>
-      <c r="F35" s="170" t="s">
+      <c r="F35" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="174" t="s">
+      <c r="G35" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="175"/>
-      <c r="I35" s="182" t="s">
+      <c r="H35" s="168"/>
+      <c r="I35" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="175"/>
-      <c r="K35" s="167" t="s">
+      <c r="J35" s="168"/>
+      <c r="K35" s="164" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="184" t="s">
+      <c r="L35" s="171" t="s">
         <v>22</v>
       </c>
-      <c r="M35" s="186" t="s">
+      <c r="M35" s="173" t="s">
         <v>27</v>
       </c>
-      <c r="N35" s="181" t="s">
+      <c r="N35" s="163" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="66"/>
-      <c r="C36" s="166"/>
-      <c r="D36" s="166"/>
-      <c r="E36" s="167"/>
-      <c r="F36" s="170"/>
-      <c r="G36" s="176"/>
-      <c r="H36" s="177"/>
-      <c r="I36" s="183"/>
-      <c r="J36" s="177"/>
-      <c r="K36" s="167"/>
-      <c r="L36" s="185"/>
-      <c r="M36" s="181"/>
-      <c r="N36" s="167"/>
+      <c r="C36" s="180"/>
+      <c r="D36" s="180"/>
+      <c r="E36" s="164"/>
+      <c r="F36" s="183"/>
+      <c r="G36" s="188"/>
+      <c r="H36" s="170"/>
+      <c r="I36" s="169"/>
+      <c r="J36" s="170"/>
+      <c r="K36" s="164"/>
+      <c r="L36" s="172"/>
+      <c r="M36" s="163"/>
+      <c r="N36" s="164"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="66"/>
       <c r="C37" s="24">
         <v>8</v>
       </c>
-      <c r="D37" s="188">
+      <c r="D37" s="118">
         <v>1</v>
       </c>
       <c r="E37" s="25">
@@ -5409,14 +5409,14 @@
       <c r="F37" s="29">
         <v>1</v>
       </c>
-      <c r="G37" s="162">
+      <c r="G37" s="165">
         <v>1</v>
       </c>
-      <c r="H37" s="163"/>
-      <c r="I37" s="162">
+      <c r="H37" s="166"/>
+      <c r="I37" s="165">
         <v>1</v>
       </c>
-      <c r="J37" s="163"/>
+      <c r="J37" s="166"/>
       <c r="K37" s="116">
         <v>0</v>
       </c>
@@ -5444,18 +5444,18 @@
       <c r="F38" s="29">
         <v>0</v>
       </c>
-      <c r="G38" s="162">
+      <c r="G38" s="165">
         <v>0</v>
       </c>
-      <c r="H38" s="163"/>
-      <c r="I38" s="162">
+      <c r="H38" s="166"/>
+      <c r="I38" s="165">
         <v>0</v>
       </c>
-      <c r="J38" s="163"/>
+      <c r="J38" s="166"/>
       <c r="K38" s="28">
         <v>0</v>
       </c>
-      <c r="L38" s="187">
+      <c r="L38" s="117">
         <v>9</v>
       </c>
       <c r="M38" s="27">
@@ -5467,14 +5467,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I35:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="M35:M36"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
@@ -5490,6 +5482,14 @@
     <mergeCell ref="K35:K36"/>
     <mergeCell ref="G34:K34"/>
     <mergeCell ref="G35:H36"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I35:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="M35:M36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5498,21 +5498,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A33786056CB34C49BCEFA0219ACF09AA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe1a16f605cb49944c1e91188c54d23f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="63f82232-4b4a-4992-a008-0c2680091aa8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c3ae1477633211a0ddb73f406e1224d" ns2:_="">
     <xsd:import namespace="63f82232-4b4a-4992-a008-0c2680091aa8"/>
@@ -5676,24 +5661,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88DD952-A6CF-436F-8B36-51E413798B79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73A5BE66-B540-4CCE-B0F4-199F4D574EF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0B58DA-A86C-4275-91CE-56836C8F6B2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5709,4 +5692,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73A5BE66-B540-4CCE-B0F4-199F4D574EF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88DD952-A6CF-436F-8B36-51E413798B79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update excel file, update EmployeeMockTest
</commit_message>
<xml_diff>
--- a/Docs/Lab3/Lab03_BBT_TCs_Form.xlsx
+++ b/Docs/Lab3/Lab03_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0371C9F7-0968-4A20-A201-B8F459B19B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AD8309-14F2-4EEA-8B9B-A7D63BD238D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cerinta" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="111">
   <si>
     <t>Condition</t>
   </si>
@@ -354,9 +354,6 @@
   </si>
   <si>
     <t>1, 5</t>
-  </si>
-  <si>
-    <t>firstName începe cu literă mică, sau cu un caracter care nu este de tip literă.(6)</t>
   </si>
   <si>
     <r>
@@ -597,6 +594,12 @@
   </si>
   <si>
     <t>run2</t>
+  </si>
+  <si>
+    <t>firstName începe cu literă mică, sau cu un caracter care nu este de tip literă</t>
+  </si>
+  <si>
+    <t>Angajatul a fost adăugat cu succes.</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1647,6 +1650,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1683,44 +1722,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1737,11 +1743,68 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1755,27 +1818,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1785,50 +1833,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2047,7 +2053,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>121626</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>137161</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2091,7 +2097,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>683455</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>142892</xdr:rowOff>
+      <xdr:rowOff>142893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2135,7 +2141,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1112462</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>144781</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2634,7 +2640,7 @@
   </sheetPr>
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -2819,8 +2825,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="F2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,49 +2876,49 @@
       <c r="H3" s="90"/>
     </row>
     <row r="5" spans="2:17" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="130" t="s">
+      <c r="B5" s="142" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="H5" s="131" t="s">
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="H5" s="143" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
     </row>
     <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="130"/>
-      <c r="C6" s="130"/>
-      <c r="D6" s="130"/>
-      <c r="E6" s="130"/>
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="144"/>
+      <c r="J6" s="144"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G7" s="133" t="s">
+      <c r="G7" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="135" t="s">
+      <c r="H7" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="144" t="s">
+      <c r="I7" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="145"/>
-      <c r="K7" s="145"/>
-      <c r="L7" s="145"/>
-      <c r="M7" s="145"/>
-      <c r="N7" s="145"/>
-      <c r="O7" s="146"/>
-      <c r="P7" s="147" t="s">
+      <c r="J7" s="135"/>
+      <c r="K7" s="135"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="135"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="147"/>
+      <c r="Q7" s="137"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
@@ -2927,37 +2933,37 @@
       <c r="E8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="134"/>
-      <c r="H8" s="136"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="148"/>
       <c r="I8" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="L8" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="96" t="s">
+      <c r="M8" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="N8" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="N8" s="144" t="s">
-        <v>72</v>
-      </c>
-      <c r="O8" s="146"/>
-      <c r="P8" s="144" t="s">
+      <c r="O8" s="136"/>
+      <c r="P8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="Q8" s="146"/>
+      <c r="Q8" s="136"/>
     </row>
     <row r="9" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="84">
         <v>1</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="C9" s="149" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="98" t="s">
@@ -2974,31 +2980,31 @@
         <v>1</v>
       </c>
       <c r="J9" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" s="102" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="102" t="s">
-        <v>73</v>
-      </c>
-      <c r="M9" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" s="140">
+      <c r="N9" s="128">
         <v>3000</v>
       </c>
-      <c r="O9" s="141"/>
-      <c r="P9" s="142" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q9" s="143"/>
+      <c r="O9" s="129"/>
+      <c r="P9" s="132" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9" s="133"/>
     </row>
     <row r="10" spans="2:17" s="66" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="84">
         <v>2</v>
       </c>
-      <c r="C10" s="138"/>
+      <c r="C10" s="150"/>
       <c r="D10" s="98"/>
       <c r="E10" s="99" t="s">
         <v>56</v>
@@ -3007,29 +3013,29 @@
         <v>2</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" s="38">
         <v>1</v>
       </c>
       <c r="J10" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="102" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" s="38" t="s">
         <v>75</v>
-      </c>
-      <c r="K10" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="L10" s="102" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10" s="38" t="s">
-        <v>76</v>
       </c>
       <c r="N10" s="93">
         <v>3000</v>
       </c>
       <c r="O10" s="94"/>
       <c r="P10" s="103" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q10" s="95"/>
     </row>
@@ -3037,7 +3043,7 @@
       <c r="B11" s="84">
         <v>3</v>
       </c>
-      <c r="C11" s="138"/>
+      <c r="C11" s="150"/>
       <c r="D11" s="97"/>
       <c r="E11" s="99" t="s">
         <v>58</v>
@@ -3046,29 +3052,29 @@
         <v>3</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I11" s="38">
         <v>1</v>
       </c>
       <c r="J11" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="38" t="s">
         <v>75</v>
-      </c>
-      <c r="K11" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="L11" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="M11" s="38" t="s">
-        <v>76</v>
       </c>
       <c r="N11" s="93">
         <v>3000</v>
       </c>
       <c r="O11" s="94"/>
       <c r="P11" s="103" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q11" s="95"/>
     </row>
@@ -3076,7 +3082,7 @@
       <c r="B12" s="84">
         <v>4</v>
       </c>
-      <c r="C12" s="139"/>
+      <c r="C12" s="151"/>
       <c r="D12" s="84"/>
       <c r="E12" s="99" t="s">
         <v>57</v>
@@ -3085,82 +3091,82 @@
         <v>4</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I12" s="20">
         <v>1</v>
       </c>
       <c r="J12" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="K12" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="M12" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="N12" s="140">
+      <c r="N12" s="128">
         <v>3000</v>
       </c>
-      <c r="O12" s="141"/>
-      <c r="P12" s="148" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q12" s="149"/>
-    </row>
-    <row r="13" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O12" s="129"/>
+      <c r="P12" s="138" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12" s="139"/>
+    </row>
+    <row r="13" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="84">
         <v>5</v>
       </c>
-      <c r="C13" s="137" t="s">
+      <c r="C13" s="149" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="100" t="s">
-        <v>62</v>
-      </c>
+      <c r="E13" s="100"/>
       <c r="G13" s="21">
         <v>5</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13" s="20">
         <v>1</v>
       </c>
       <c r="J13" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="102" t="s">
+        <v>91</v>
+      </c>
+      <c r="M13" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="102" t="s">
-        <v>92</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="N13" s="140">
+      <c r="N13" s="128">
         <v>3000</v>
       </c>
-      <c r="O13" s="141"/>
-      <c r="P13" s="148" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q13" s="141"/>
-    </row>
-    <row r="14" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="129"/>
+      <c r="P13" s="138" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q13" s="129"/>
+    </row>
+    <row r="14" spans="2:17" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="84">
         <v>6</v>
       </c>
-      <c r="C14" s="139"/>
+      <c r="C14" s="151"/>
       <c r="D14" s="84"/>
-      <c r="E14" s="99"/>
+      <c r="E14" s="99" t="s">
+        <v>109</v>
+      </c>
       <c r="G14" s="21">
         <v>6</v>
       </c>
@@ -3170,16 +3176,16 @@
       <c r="K14" s="20"/>
       <c r="L14" s="38"/>
       <c r="M14" s="20"/>
-      <c r="N14" s="140"/>
-      <c r="O14" s="141"/>
-      <c r="P14" s="140"/>
-      <c r="Q14" s="141"/>
+      <c r="N14" s="128"/>
+      <c r="O14" s="129"/>
+      <c r="P14" s="128"/>
+      <c r="Q14" s="129"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="84">
         <v>7</v>
       </c>
-      <c r="C15" s="128"/>
+      <c r="C15" s="140"/>
       <c r="D15" s="84"/>
       <c r="E15" s="84"/>
       <c r="G15" s="21">
@@ -3191,16 +3197,16 @@
       <c r="K15" s="20"/>
       <c r="L15" s="38"/>
       <c r="M15" s="20"/>
-      <c r="N15" s="140"/>
-      <c r="O15" s="141"/>
-      <c r="P15" s="140"/>
-      <c r="Q15" s="141"/>
+      <c r="N15" s="128"/>
+      <c r="O15" s="129"/>
+      <c r="P15" s="128"/>
+      <c r="Q15" s="129"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="84">
         <v>8</v>
       </c>
-      <c r="C16" s="129"/>
+      <c r="C16" s="141"/>
       <c r="D16" s="84"/>
       <c r="E16" s="84"/>
       <c r="G16" s="21">
@@ -3212,16 +3218,16 @@
       <c r="K16" s="20"/>
       <c r="L16" s="38"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="140"/>
-      <c r="O16" s="141"/>
-      <c r="P16" s="140"/>
-      <c r="Q16" s="141"/>
+      <c r="N16" s="128"/>
+      <c r="O16" s="129"/>
+      <c r="P16" s="128"/>
+      <c r="Q16" s="129"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" s="84">
         <v>9</v>
       </c>
-      <c r="C17" s="128"/>
+      <c r="C17" s="140"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
       <c r="G17" s="21">
@@ -3233,16 +3239,16 @@
       <c r="K17" s="20"/>
       <c r="L17" s="38"/>
       <c r="M17" s="20"/>
-      <c r="N17" s="140"/>
-      <c r="O17" s="141"/>
-      <c r="P17" s="142"/>
-      <c r="Q17" s="143"/>
+      <c r="N17" s="128"/>
+      <c r="O17" s="129"/>
+      <c r="P17" s="132"/>
+      <c r="Q17" s="133"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B18" s="84">
         <v>10</v>
       </c>
-      <c r="C18" s="129"/>
+      <c r="C18" s="141"/>
       <c r="D18" s="84"/>
       <c r="E18" s="84"/>
       <c r="G18" s="21"/>
@@ -3252,16 +3258,16 @@
       <c r="K18" s="20"/>
       <c r="L18" s="38"/>
       <c r="M18" s="20"/>
-      <c r="N18" s="140"/>
-      <c r="O18" s="141"/>
-      <c r="P18" s="140"/>
-      <c r="Q18" s="141"/>
+      <c r="N18" s="128"/>
+      <c r="O18" s="129"/>
+      <c r="P18" s="128"/>
+      <c r="Q18" s="129"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="84">
         <v>11</v>
       </c>
-      <c r="C19" s="128"/>
+      <c r="C19" s="140"/>
       <c r="D19" s="84"/>
       <c r="E19" s="84"/>
       <c r="G19" s="11"/>
@@ -3271,16 +3277,16 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="140"/>
-      <c r="O19" s="141"/>
-      <c r="P19" s="150"/>
-      <c r="Q19" s="151"/>
+      <c r="N19" s="128"/>
+      <c r="O19" s="129"/>
+      <c r="P19" s="130"/>
+      <c r="Q19" s="131"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" s="84">
         <v>12</v>
       </c>
-      <c r="C20" s="129"/>
+      <c r="C20" s="141"/>
       <c r="D20" s="84"/>
       <c r="E20" s="84"/>
       <c r="G20" s="11"/>
@@ -3290,16 +3296,16 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="140"/>
-      <c r="O20" s="141"/>
-      <c r="P20" s="150"/>
-      <c r="Q20" s="151"/>
+      <c r="N20" s="128"/>
+      <c r="O20" s="129"/>
+      <c r="P20" s="130"/>
+      <c r="Q20" s="131"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="84">
         <v>13</v>
       </c>
-      <c r="C21" s="128"/>
+      <c r="C21" s="140"/>
       <c r="D21" s="84"/>
       <c r="E21" s="84"/>
       <c r="G21" s="11"/>
@@ -3309,16 +3315,16 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="140"/>
-      <c r="O21" s="141"/>
-      <c r="P21" s="150"/>
-      <c r="Q21" s="151"/>
+      <c r="N21" s="128"/>
+      <c r="O21" s="129"/>
+      <c r="P21" s="130"/>
+      <c r="Q21" s="131"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" s="84">
         <v>14</v>
       </c>
-      <c r="C22" s="129"/>
+      <c r="C22" s="141"/>
       <c r="D22" s="84"/>
       <c r="E22" s="84"/>
       <c r="G22" s="14"/>
@@ -3328,16 +3334,16 @@
       <c r="K22" s="20"/>
       <c r="L22" s="38"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="140"/>
-      <c r="O22" s="141"/>
-      <c r="P22" s="150"/>
-      <c r="Q22" s="151"/>
+      <c r="N22" s="128"/>
+      <c r="O22" s="129"/>
+      <c r="P22" s="130"/>
+      <c r="Q22" s="131"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" s="84">
         <v>15</v>
       </c>
-      <c r="C23" s="128"/>
+      <c r="C23" s="140"/>
       <c r="D23" s="84"/>
       <c r="E23" s="84"/>
     </row>
@@ -3345,7 +3351,7 @@
       <c r="B24" s="84">
         <v>16</v>
       </c>
-      <c r="C24" s="129"/>
+      <c r="C24" s="141"/>
       <c r="D24" s="84"/>
       <c r="E24" s="84"/>
     </row>
@@ -3452,18 +3458,18 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="H5:J6"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="P17:Q17"/>
@@ -3480,18 +3486,18 @@
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N13:O13"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="H5:J6"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3506,7 +3512,7 @@
   </sheetPr>
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -3556,57 +3562,57 @@
       <c r="J4" s="77"/>
     </row>
     <row r="5" spans="2:18" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="156" t="s">
+      <c r="B5" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="H5" s="131" t="s">
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
+      <c r="H5" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
     </row>
     <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="157"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="157"/>
-      <c r="E6" s="157"/>
+      <c r="B6" s="158"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="131"/>
-      <c r="M6" s="131"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="143"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="143"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
     </row>
     <row r="7" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F7" s="5"/>
-      <c r="H7" s="133" t="s">
+      <c r="H7" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="133" t="s">
+      <c r="I7" s="145" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="133" t="s">
+      <c r="J7" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="135" t="s">
+      <c r="K7" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="153" t="s">
+      <c r="L7" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="154"/>
-      <c r="N7" s="154"/>
-      <c r="O7" s="154"/>
-      <c r="P7" s="154"/>
-      <c r="Q7" s="155"/>
+      <c r="M7" s="155"/>
+      <c r="N7" s="155"/>
+      <c r="O7" s="155"/>
+      <c r="P7" s="155"/>
+      <c r="Q7" s="156"/>
       <c r="R7" s="86" t="s">
         <v>6</v>
       </c>
@@ -3618,49 +3624,49 @@
       <c r="C8" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="144" t="s">
+      <c r="D8" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="146"/>
+      <c r="E8" s="136"/>
       <c r="F8" s="3"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="136"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="148"/>
       <c r="L8" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="N8" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="30" t="s">
+      <c r="O8" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="O8" s="30" t="s">
+      <c r="P8" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="P8" s="96" t="s">
+      <c r="Q8" s="30" t="s">
         <v>71</v>
-      </c>
-      <c r="Q8" s="30" t="s">
-        <v>72</v>
       </c>
       <c r="R8" s="83" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="C9" s="149" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="84">
         <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="3"/>
       <c r="H9" s="82">
@@ -3670,41 +3676,41 @@
         <v>1</v>
       </c>
       <c r="J9" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="71" t="s">
         <v>89</v>
-      </c>
-      <c r="K9" s="71" t="s">
-        <v>90</v>
       </c>
       <c r="L9" s="71">
         <v>1</v>
       </c>
       <c r="M9" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="P9" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="N9" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="O9" s="106" t="s">
-        <v>81</v>
-      </c>
-      <c r="P9" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="Q9" s="71">
         <v>3000</v>
       </c>
       <c r="R9" s="105" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="152"/>
-      <c r="C10" s="138"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="150"/>
       <c r="D10" s="84">
         <v>2</v>
       </c>
       <c r="E10" s="101" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="3"/>
       <c r="H10" s="82">
@@ -3714,41 +3720,41 @@
         <v>2</v>
       </c>
       <c r="J10" s="71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K10" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L10" s="71">
         <v>1</v>
       </c>
       <c r="M10" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="P10" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="N10" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="O10" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="P10" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="Q10" s="71">
         <v>3000</v>
       </c>
       <c r="R10" s="107" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="152"/>
-      <c r="C11" s="138"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="150"/>
       <c r="D11" s="84">
         <v>3</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" s="3"/>
       <c r="H11" s="82">
@@ -3758,36 +3764,36 @@
         <v>3</v>
       </c>
       <c r="J11" s="71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K11" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L11" s="71">
         <v>1</v>
       </c>
       <c r="M11" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="P11" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="N11" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="O11" s="106" t="s">
-        <v>92</v>
-      </c>
-      <c r="P11" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="Q11" s="71">
         <v>3000</v>
       </c>
       <c r="R11" s="104" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="152"/>
-      <c r="C12" s="138"/>
+      <c r="B12" s="159"/>
+      <c r="C12" s="150"/>
       <c r="D12" s="84">
         <v>4</v>
       </c>
@@ -3810,8 +3816,8 @@
       <c r="R12" s="71"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="152"/>
-      <c r="C13" s="138"/>
+      <c r="B13" s="159"/>
+      <c r="C13" s="150"/>
       <c r="D13" s="84">
         <v>5</v>
       </c>
@@ -3834,8 +3840,8 @@
       <c r="R13" s="71"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="129"/>
-      <c r="C14" s="139"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="151"/>
       <c r="D14" s="84">
         <v>6</v>
       </c>
@@ -3858,17 +3864,17 @@
       <c r="R14" s="71"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="137" t="s">
+      <c r="C15" s="149" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="84">
         <v>7</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" s="3"/>
       <c r="H15" s="82">
@@ -3878,41 +3884,41 @@
         <v>7</v>
       </c>
       <c r="J15" s="106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L15" s="71">
         <v>1</v>
       </c>
       <c r="M15" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15" s="106" t="s">
+        <v>93</v>
+      </c>
+      <c r="O15" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="N15" s="106" t="s">
-        <v>94</v>
-      </c>
-      <c r="O15" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="P15" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="Q15" s="71">
         <v>3000</v>
       </c>
       <c r="R15" s="105" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="152"/>
-      <c r="C16" s="138"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="150"/>
       <c r="D16" s="84">
         <v>8</v>
       </c>
       <c r="E16" s="101" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" s="3"/>
       <c r="H16" s="82">
@@ -3922,41 +3928,41 @@
         <v>8</v>
       </c>
       <c r="J16" s="106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K16" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L16" s="71">
         <v>1</v>
       </c>
       <c r="M16" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="O16" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="P16" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="N16" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="O16" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="P16" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="Q16" s="71">
         <v>3000</v>
       </c>
       <c r="R16" s="107" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="152"/>
-      <c r="C17" s="138"/>
+      <c r="B17" s="159"/>
+      <c r="C17" s="150"/>
       <c r="D17" s="84">
         <v>9</v>
       </c>
       <c r="E17" s="101" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" s="3"/>
       <c r="H17" s="82">
@@ -3966,41 +3972,41 @@
         <v>9</v>
       </c>
       <c r="J17" s="106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K17" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L17" s="71">
         <v>1</v>
       </c>
       <c r="M17" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="O17" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="N17" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="O17" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="P17" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="Q17" s="71">
         <v>3000</v>
       </c>
       <c r="R17" s="107" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="152"/>
-      <c r="C18" s="138"/>
+      <c r="B18" s="159"/>
+      <c r="C18" s="150"/>
       <c r="D18" s="84">
         <v>10</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F18" s="3"/>
       <c r="H18" s="82">
@@ -4010,36 +4016,36 @@
         <v>10</v>
       </c>
       <c r="J18" s="106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K18" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L18" s="71">
         <v>1</v>
       </c>
       <c r="M18" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="O18" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="P18" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="N18" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="O18" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="P18" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="Q18" s="71">
         <v>3000</v>
       </c>
       <c r="R18" s="104" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="152"/>
-      <c r="C19" s="138"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="150"/>
       <c r="D19" s="84">
         <v>11</v>
       </c>
@@ -4062,8 +4068,8 @@
       <c r="R19" s="71"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="129"/>
-      <c r="C20" s="139"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="151"/>
       <c r="D20" s="84">
         <v>12</v>
       </c>
@@ -4086,10 +4092,10 @@
       <c r="R20" s="72"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="128"/>
+      <c r="C21" s="140"/>
       <c r="D21" s="84">
         <v>13</v>
       </c>
@@ -4112,8 +4118,8 @@
       <c r="R21" s="72"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="152"/>
-      <c r="C22" s="152"/>
+      <c r="B22" s="159"/>
+      <c r="C22" s="159"/>
       <c r="D22" s="84">
         <v>14</v>
       </c>
@@ -4136,8 +4142,8 @@
       <c r="R22" s="72"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="152"/>
-      <c r="C23" s="152"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
       <c r="D23" s="84">
         <v>15</v>
       </c>
@@ -4160,8 +4166,8 @@
       <c r="R23" s="71"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B24" s="152"/>
-      <c r="C24" s="152"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="159"/>
       <c r="D24" s="84">
         <v>16</v>
       </c>
@@ -4184,8 +4190,8 @@
       <c r="R24" s="71"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="152"/>
-      <c r="C25" s="152"/>
+      <c r="B25" s="159"/>
+      <c r="C25" s="159"/>
       <c r="D25" s="84">
         <v>17</v>
       </c>
@@ -4208,8 +4214,8 @@
       <c r="R25" s="71"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="129"/>
-      <c r="C26" s="129"/>
+      <c r="B26" s="141"/>
+      <c r="C26" s="141"/>
       <c r="D26" s="84">
         <v>18</v>
       </c>
@@ -4232,10 +4238,10 @@
       <c r="R26" s="72"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="128" t="s">
+      <c r="B27" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="128"/>
+      <c r="C27" s="140"/>
       <c r="D27" s="84">
         <v>19</v>
       </c>
@@ -4259,8 +4265,8 @@
       <c r="S27" s="3"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B28" s="152"/>
-      <c r="C28" s="152"/>
+      <c r="B28" s="159"/>
+      <c r="C28" s="159"/>
       <c r="D28" s="84">
         <v>20</v>
       </c>
@@ -4284,8 +4290,8 @@
       <c r="S28" s="3"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="152"/>
-      <c r="C29" s="152"/>
+      <c r="B29" s="159"/>
+      <c r="C29" s="159"/>
       <c r="D29" s="84">
         <v>21</v>
       </c>
@@ -4309,8 +4315,8 @@
       <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B30" s="152"/>
-      <c r="C30" s="152"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
       <c r="D30" s="84">
         <v>22</v>
       </c>
@@ -4334,8 +4340,8 @@
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="152"/>
-      <c r="C31" s="152"/>
+      <c r="B31" s="159"/>
+      <c r="C31" s="159"/>
       <c r="D31" s="84">
         <v>23</v>
       </c>
@@ -4358,8 +4364,8 @@
       <c r="R31" s="71"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="129"/>
-      <c r="C32" s="129"/>
+      <c r="B32" s="141"/>
+      <c r="C32" s="141"/>
       <c r="D32" s="84">
         <v>24</v>
       </c>
@@ -4381,10 +4387,10 @@
       <c r="R32" s="72"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B33" s="128" t="s">
+      <c r="B33" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="128"/>
+      <c r="C33" s="140"/>
       <c r="D33" s="84">
         <v>25</v>
       </c>
@@ -4406,8 +4412,8 @@
       <c r="R33" s="87"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B34" s="152"/>
-      <c r="C34" s="152"/>
+      <c r="B34" s="159"/>
+      <c r="C34" s="159"/>
       <c r="D34" s="84">
         <v>26</v>
       </c>
@@ -4429,8 +4435,8 @@
       <c r="R34" s="72"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
       <c r="D35" s="84">
         <v>27</v>
       </c>
@@ -4452,8 +4458,8 @@
       <c r="R35" s="71"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B36" s="152"/>
-      <c r="C36" s="152"/>
+      <c r="B36" s="159"/>
+      <c r="C36" s="159"/>
       <c r="D36" s="84">
         <v>28</v>
       </c>
@@ -4475,8 +4481,8 @@
       <c r="R36" s="71"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B37" s="152"/>
-      <c r="C37" s="152"/>
+      <c r="B37" s="159"/>
+      <c r="C37" s="159"/>
       <c r="D37" s="84">
         <v>29</v>
       </c>
@@ -4498,8 +4504,8 @@
       <c r="R37" s="71"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="129"/>
-      <c r="C38" s="129"/>
+      <c r="B38" s="141"/>
+      <c r="C38" s="141"/>
       <c r="D38" s="84">
         <v>30</v>
       </c>
@@ -4524,8 +4530,8 @@
       <c r="A40" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="H40" s="158"/>
-      <c r="I40" s="159"/>
+      <c r="H40" s="152"/>
+      <c r="I40" s="153"/>
       <c r="J40" s="66"/>
       <c r="K40" s="66"/>
       <c r="L40" s="66"/>
@@ -4562,16 +4568,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="L7:Q7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="H5:M6"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="B33:B38"/>
@@ -4582,6 +4578,16 @@
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="C21:C26"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="H5:M6"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4596,8 +4602,8 @@
   </sheetPr>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4612,7 +4618,7 @@
     <col min="9" max="9" width="14" style="66" customWidth="1"/>
     <col min="10" max="10" width="9.21875" customWidth="1"/>
     <col min="11" max="11" width="19.88671875" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4634,72 +4640,72 @@
     </row>
     <row r="3" spans="2:13" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22"/>
-      <c r="C3" s="181" t="s">
+      <c r="C3" s="170" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-      <c r="E4" s="182"/>
-      <c r="F4" s="182"/>
-      <c r="G4" s="182"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
       <c r="L4" s="115" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M4" s="115" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="175" t="s">
+      <c r="C5" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="145"/>
-      <c r="K5" s="146"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="136"/>
       <c r="L5" s="88" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="66"/>
     </row>
     <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="174"/>
-      <c r="C6" s="176"/>
-      <c r="D6" s="177"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="163"/>
       <c r="E6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="G6" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="I6" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="J6" s="37" t="s">
         <v>71</v>
-      </c>
-      <c r="J6" s="37" t="s">
-        <v>72</v>
       </c>
       <c r="K6" s="33" t="s">
         <v>7</v>
@@ -4714,37 +4720,37 @@
         <v>1</v>
       </c>
       <c r="C7" s="110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="108">
         <v>1</v>
       </c>
       <c r="F7" s="108" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="112" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="108" t="s">
         <v>75</v>
-      </c>
-      <c r="G7" s="108" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="112" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="108" t="s">
-        <v>76</v>
       </c>
       <c r="J7" s="93">
         <v>3000</v>
       </c>
       <c r="K7" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" s="103" t="b">
         <v>1</v>
       </c>
       <c r="M7" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -4752,37 +4758,37 @@
         <v>2</v>
       </c>
       <c r="C8" s="111" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="108">
         <v>1</v>
       </c>
       <c r="F8" s="108" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="108" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="108" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="108" t="s">
         <v>75</v>
-      </c>
-      <c r="G8" s="108" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="108" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" s="108" t="s">
-        <v>76</v>
       </c>
       <c r="J8" s="93">
         <v>3000</v>
       </c>
       <c r="K8" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L8" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M8" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -4790,37 +4796,37 @@
         <v>3</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="71">
         <v>1</v>
       </c>
       <c r="F9" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="G9" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="106" t="s">
-        <v>81</v>
-      </c>
-      <c r="I9" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="J9" s="71">
         <v>3000</v>
       </c>
       <c r="K9" s="105" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L9" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M9" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:13" s="34" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4828,34 +4834,34 @@
         <v>4</v>
       </c>
       <c r="C10" s="71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" s="71">
         <v>1</v>
       </c>
       <c r="F10" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="G10" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="J10" s="71">
         <v>3000</v>
       </c>
       <c r="K10" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L10" s="103" t="b">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="L10" s="189" t="s">
+        <v>110</v>
       </c>
       <c r="M10" s="103" t="b">
         <v>1</v>
@@ -4866,37 +4872,37 @@
         <v>5</v>
       </c>
       <c r="C11" s="71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" s="71">
         <v>1</v>
       </c>
       <c r="F11" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="G11" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="106" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="J11" s="71">
         <v>3000</v>
       </c>
       <c r="K11" s="104" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L11" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M11" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:13" s="34" customFormat="1" x14ac:dyDescent="0.3">
@@ -4904,37 +4910,37 @@
         <v>6</v>
       </c>
       <c r="C12" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="84" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" s="71">
         <v>1</v>
       </c>
       <c r="F12" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="106" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="G12" s="106" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="I12" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="J12" s="71">
         <v>3000</v>
       </c>
       <c r="K12" s="105" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L12" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M12" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:13" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4942,34 +4948,34 @@
         <v>7</v>
       </c>
       <c r="C13" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" s="71">
         <v>1</v>
       </c>
       <c r="F13" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="G13" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="J13" s="71">
         <v>3000</v>
       </c>
       <c r="K13" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" s="103" t="b">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="L13" s="189" t="s">
+        <v>110</v>
       </c>
       <c r="M13" s="103" t="b">
         <v>1</v>
@@ -4980,34 +4986,34 @@
         <v>8</v>
       </c>
       <c r="C14" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="84" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="71">
         <v>1</v>
       </c>
       <c r="F14" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="G14" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="J14" s="71">
         <v>3000</v>
       </c>
       <c r="K14" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L14" s="103" t="b">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="L14" s="189" t="s">
+        <v>110</v>
       </c>
       <c r="M14" s="103" t="b">
         <v>1</v>
@@ -5018,37 +5024,37 @@
         <v>9</v>
       </c>
       <c r="C15" s="109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" s="71">
         <v>1</v>
       </c>
       <c r="F15" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="71" t="s">
         <v>75</v>
-      </c>
-      <c r="G15" s="106" t="s">
-        <v>108</v>
-      </c>
-      <c r="H15" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" s="71" t="s">
-        <v>76</v>
       </c>
       <c r="J15" s="71">
         <v>3000</v>
       </c>
       <c r="K15" s="104" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L15" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M15" s="113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
@@ -5326,74 +5332,74 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="178"/>
-      <c r="D34" s="178"/>
-      <c r="E34" s="179"/>
+      <c r="C34" s="166"/>
+      <c r="D34" s="166"/>
+      <c r="E34" s="167"/>
       <c r="F34" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="184" t="s">
+      <c r="G34" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="185"/>
-      <c r="I34" s="185"/>
-      <c r="J34" s="178"/>
-      <c r="K34" s="186"/>
-      <c r="L34" s="160" t="s">
+      <c r="H34" s="174"/>
+      <c r="I34" s="174"/>
+      <c r="J34" s="166"/>
+      <c r="K34" s="175"/>
+      <c r="L34" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="M34" s="161"/>
-      <c r="N34" s="162"/>
+      <c r="M34" s="181"/>
+      <c r="N34" s="182"/>
     </row>
     <row r="35" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="66"/>
-      <c r="C35" s="180" t="s">
+      <c r="C35" s="168" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="180" t="s">
+      <c r="D35" s="168" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="164" t="s">
+      <c r="E35" s="169" t="s">
         <v>21</v>
       </c>
-      <c r="F35" s="183" t="s">
+      <c r="F35" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="187" t="s">
+      <c r="G35" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="168"/>
-      <c r="I35" s="167" t="s">
+      <c r="H35" s="177"/>
+      <c r="I35" s="184" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="168"/>
-      <c r="K35" s="164" t="s">
+      <c r="J35" s="177"/>
+      <c r="K35" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="171" t="s">
+      <c r="L35" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="M35" s="173" t="s">
+      <c r="M35" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="N35" s="163" t="s">
-        <v>107</v>
+      <c r="N35" s="183" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="66"/>
-      <c r="C36" s="180"/>
-      <c r="D36" s="180"/>
-      <c r="E36" s="164"/>
-      <c r="F36" s="183"/>
-      <c r="G36" s="188"/>
-      <c r="H36" s="170"/>
-      <c r="I36" s="169"/>
-      <c r="J36" s="170"/>
-      <c r="K36" s="164"/>
-      <c r="L36" s="172"/>
-      <c r="M36" s="163"/>
-      <c r="N36" s="164"/>
+      <c r="C36" s="168"/>
+      <c r="D36" s="168"/>
+      <c r="E36" s="169"/>
+      <c r="F36" s="172"/>
+      <c r="G36" s="178"/>
+      <c r="H36" s="179"/>
+      <c r="I36" s="185"/>
+      <c r="J36" s="179"/>
+      <c r="K36" s="169"/>
+      <c r="L36" s="187"/>
+      <c r="M36" s="183"/>
+      <c r="N36" s="169"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="66"/>
@@ -5409,22 +5415,22 @@
       <c r="F37" s="29">
         <v>1</v>
       </c>
-      <c r="G37" s="165">
+      <c r="G37" s="164">
         <v>1</v>
       </c>
-      <c r="H37" s="166"/>
-      <c r="I37" s="165">
+      <c r="H37" s="165"/>
+      <c r="I37" s="164">
         <v>1</v>
       </c>
-      <c r="J37" s="166"/>
+      <c r="J37" s="165"/>
       <c r="K37" s="116">
         <v>0</v>
       </c>
       <c r="L37" s="28">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M37" s="27">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="N37" s="25">
         <v>0</v>
@@ -5432,41 +5438,29 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="66"/>
-      <c r="C38" s="114">
-        <v>9</v>
-      </c>
-      <c r="D38" s="27">
-        <v>0</v>
-      </c>
-      <c r="E38" s="25">
-        <v>0</v>
-      </c>
-      <c r="F38" s="29">
-        <v>0</v>
-      </c>
-      <c r="G38" s="165">
-        <v>0</v>
-      </c>
-      <c r="H38" s="166"/>
-      <c r="I38" s="165">
-        <v>0</v>
-      </c>
-      <c r="J38" s="166"/>
-      <c r="K38" s="28">
-        <v>0</v>
-      </c>
-      <c r="L38" s="117">
-        <v>9</v>
-      </c>
-      <c r="M38" s="27">
-        <v>9</v>
-      </c>
-      <c r="N38" s="25">
-        <v>0</v>
-      </c>
+      <c r="C38" s="114"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="164"/>
+      <c r="H38" s="165"/>
+      <c r="I38" s="164"/>
+      <c r="J38" s="165"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="117"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I35:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="M35:M36"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
@@ -5482,14 +5476,6 @@
     <mergeCell ref="K35:K36"/>
     <mergeCell ref="G34:K34"/>
     <mergeCell ref="G35:H36"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I35:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="M35:M36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5498,6 +5484,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A33786056CB34C49BCEFA0219ACF09AA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe1a16f605cb49944c1e91188c54d23f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="63f82232-4b4a-4992-a008-0c2680091aa8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c3ae1477633211a0ddb73f406e1224d" ns2:_="">
     <xsd:import namespace="63f82232-4b4a-4992-a008-0c2680091aa8"/>
@@ -5661,22 +5662,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88DD952-A6CF-436F-8B36-51E413798B79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73A5BE66-B540-4CCE-B0F4-199F4D574EF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0B58DA-A86C-4275-91CE-56836C8F6B2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5692,21 +5695,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73A5BE66-B540-4CCE-B0F4-199F4D574EF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88DD952-A6CF-436F-8B36-51E413798B79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>